<commit_message>
Shear center calcualations verified
</commit_message>
<xml_diff>
--- a/Elements.xlsx
+++ b/Elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnwob\GitHub\ShearFlowThinSections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF53E7B-2666-445D-B567-2BAE0DBC52DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0113F3A2-DEE1-49FC-8044-E39E0709DB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="7020" windowWidth="26835" windowHeight="16200" xr2:uid="{164C7E60-DEC9-4E1C-9506-A74F76B88829}"/>
+    <workbookView xWindow="16125" yWindow="4245" windowWidth="28800" windowHeight="15885" xr2:uid="{164C7E60-DEC9-4E1C-9506-A74F76B88829}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>